<commit_message>
Add Shriver Center to Student/Administrative
Adds "Shriver Center" to Student Services and "Shriver Center Business Services" to Administrative Services.
</commit_message>
<xml_diff>
--- a/administrative/administrativeConfig/administrative_CategoryInfo.xlsx
+++ b/administrative/administrativeConfig/administrative_CategoryInfo.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27518"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/allyhepp/Library/Application Support/Box/Box Edit/Documents/1326468414062/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{FAFB7B40-CECC-774D-9701-6E6270227B26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E71E8D0B-D0A7-475B-B32E-81E3D683BDB1}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3546CD5-A7CD-3E45-9004-E7A8ED3B49F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38720" yWindow="680" windowWidth="34500" windowHeight="19080" xr2:uid="{27652783-9591-D547-A61D-838C8737DB69}"/>
+    <workbookView xWindow="340" yWindow="2200" windowWidth="37100" windowHeight="16700" xr2:uid="{27652783-9591-D547-A61D-838C8737DB69}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="603" uniqueCount="283">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="602" uniqueCount="284">
   <si>
     <t>Request Type Category</t>
   </si>
@@ -827,30 +827,6 @@
     <t>https://dps.umbc.edu/it-systems/</t>
   </si>
   <si>
-    <t>Adhoc IXL Contract Builder</t>
-  </si>
-  <si>
-    <t>https://my.umbc.edu/go/1187</t>
-  </si>
-  <si>
-    <t>Agreement for CLDR and AFST</t>
-  </si>
-  <si>
-    <t>https://my.umbc.edu/go/708</t>
-  </si>
-  <si>
-    <t>Agreement for CLDR and SAHAP</t>
-  </si>
-  <si>
-    <t>https://my.umbc.edu/go/709</t>
-  </si>
-  <si>
-    <t>Public Policy Pathway Agreement</t>
-  </si>
-  <si>
-    <t>https://my.umbc.edu/go/710</t>
-  </si>
-  <si>
     <t>Office of Earth &amp; Space Research Administration (ESRA)</t>
   </si>
   <si>
@@ -885,13 +861,40 @@
   </si>
   <si>
     <t>N/A</t>
+  </si>
+  <si>
+    <t>DPS Internal Documentation (DPS Employees Only)</t>
+  </si>
+  <si>
+    <t>https://umbc.atlassian.net/wiki/spaces/cps/</t>
+  </si>
+  <si>
+    <t>Shriver Center Business Services</t>
+  </si>
+  <si>
+    <t>Shriver Center New Employee Orientation</t>
+  </si>
+  <si>
+    <t>Shriver Center Business Services Forms</t>
+  </si>
+  <si>
+    <t>Shriver Center Business Services Travel Frequently Asked Questions (FAQs)</t>
+  </si>
+  <si>
+    <t>https://shriverbsu.umbc.edu/tsfaqs/</t>
+  </si>
+  <si>
+    <t>https://shriverbsu.umbc.edu/orientation/</t>
+  </si>
+  <si>
+    <t>https://shriverbsu.umbc.edu/forms/</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -976,7 +979,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -986,6 +989,9 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Good" xfId="2" builtinId="26"/>
@@ -1006,9 +1012,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1046,7 +1052,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1152,7 +1158,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1294,7 +1300,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1304,20 +1310,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0317E7B2-0780-144D-BE4D-E00A0AB6B832}">
   <dimension ref="A1:E121"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" topLeftCell="A92" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="B114" sqref="B114"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.95"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="45.375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="45.375" customWidth="1"/>
-    <col min="3" max="3" width="67.625" customWidth="1"/>
-    <col min="4" max="4" width="19.875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="93.875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="45.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="45.33203125" customWidth="1"/>
+    <col min="3" max="3" width="67.6640625" customWidth="1"/>
+    <col min="4" max="4" width="19.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="93.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1">
+    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1334,7 +1340,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" s="5" customFormat="1">
+    <row r="2" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -1351,7 +1357,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -1368,7 +1374,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -1385,7 +1391,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="15.75">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -1402,7 +1408,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -1419,7 +1425,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -1436,7 +1442,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -1453,7 +1459,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>5</v>
       </c>
@@ -1470,7 +1476,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>5</v>
       </c>
@@ -1487,7 +1493,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>5</v>
       </c>
@@ -1504,7 +1510,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>5</v>
       </c>
@@ -1521,7 +1527,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>5</v>
       </c>
@@ -1538,7 +1544,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>5</v>
       </c>
@@ -1555,7 +1561,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>5</v>
       </c>
@@ -1572,7 +1578,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>5</v>
       </c>
@@ -1589,7 +1595,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>5</v>
       </c>
@@ -1606,7 +1612,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>5</v>
       </c>
@@ -1623,7 +1629,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="19" spans="1:5">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>5</v>
       </c>
@@ -1640,7 +1646,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="20" spans="1:5">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>5</v>
       </c>
@@ -1657,7 +1663,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="21" spans="1:5">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>51</v>
       </c>
@@ -1674,7 +1680,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="22" spans="1:5">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>51</v>
       </c>
@@ -1691,7 +1697,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="23" spans="1:5">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>51</v>
       </c>
@@ -1708,7 +1714,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="24" spans="1:5">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>51</v>
       </c>
@@ -1725,7 +1731,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="25" spans="1:5">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>51</v>
       </c>
@@ -1742,7 +1748,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="26" spans="1:5">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>51</v>
       </c>
@@ -1759,7 +1765,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="27" spans="1:5">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>65</v>
       </c>
@@ -1776,7 +1782,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="28" spans="1:5">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>65</v>
       </c>
@@ -1793,7 +1799,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="29" spans="1:5">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>65</v>
       </c>
@@ -1810,7 +1816,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="30" spans="1:5">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>65</v>
       </c>
@@ -1827,7 +1833,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="31" spans="1:5">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>65</v>
       </c>
@@ -1844,7 +1850,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="32" spans="1:5">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>65</v>
       </c>
@@ -1861,7 +1867,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="33" spans="1:5">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>65</v>
       </c>
@@ -1878,7 +1884,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="34" spans="1:5">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>65</v>
       </c>
@@ -1895,7 +1901,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="35" spans="1:5">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>65</v>
       </c>
@@ -1912,7 +1918,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="36" spans="1:5">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>65</v>
       </c>
@@ -1929,7 +1935,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="37" spans="1:5">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>65</v>
       </c>
@@ -1946,7 +1952,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="38" spans="1:5">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>91</v>
       </c>
@@ -1963,7 +1969,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="39" spans="1:5">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>91</v>
       </c>
@@ -1980,7 +1986,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="40" spans="1:5">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>91</v>
       </c>
@@ -1997,7 +2003,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="41" spans="1:5">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>91</v>
       </c>
@@ -2014,7 +2020,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="42" spans="1:5">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>91</v>
       </c>
@@ -2031,7 +2037,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="43" spans="1:5">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>91</v>
       </c>
@@ -2048,7 +2054,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="44" spans="1:5">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>91</v>
       </c>
@@ -2065,7 +2071,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="45" spans="1:5">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>91</v>
       </c>
@@ -2082,7 +2088,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="46" spans="1:5">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>91</v>
       </c>
@@ -2099,7 +2105,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="47" spans="1:5">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>91</v>
       </c>
@@ -2116,7 +2122,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="48" spans="1:5">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>91</v>
       </c>
@@ -2133,7 +2139,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="49" spans="1:5">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>91</v>
       </c>
@@ -2150,7 +2156,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="50" spans="1:5">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>91</v>
       </c>
@@ -2167,7 +2173,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="51" spans="1:5">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>122</v>
       </c>
@@ -2184,7 +2190,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="52" spans="1:5">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>122</v>
       </c>
@@ -2201,7 +2207,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="53" spans="1:5">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>122</v>
       </c>
@@ -2218,7 +2224,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="54" spans="1:5">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>122</v>
       </c>
@@ -2235,7 +2241,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="55" spans="1:5">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>122</v>
       </c>
@@ -2252,7 +2258,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="56" spans="1:5">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>122</v>
       </c>
@@ -2269,7 +2275,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="57" spans="1:5">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>122</v>
       </c>
@@ -2286,7 +2292,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="58" spans="1:5">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>122</v>
       </c>
@@ -2303,7 +2309,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="59" spans="1:5">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>122</v>
       </c>
@@ -2320,7 +2326,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="60" spans="1:5">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>122</v>
       </c>
@@ -2337,7 +2343,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="61" spans="1:5">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A61" s="3" t="s">
         <v>144</v>
       </c>
@@ -2354,7 +2360,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="62" spans="1:5">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A62" s="3" t="s">
         <v>144</v>
       </c>
@@ -2371,7 +2377,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="63" spans="1:5">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A63" s="3" t="s">
         <v>144</v>
       </c>
@@ -2388,7 +2394,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="64" spans="1:5">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A64" s="3" t="s">
         <v>144</v>
       </c>
@@ -2405,7 +2411,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="65" spans="1:5">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A65" s="3" t="s">
         <v>144</v>
       </c>
@@ -2422,7 +2428,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="66" spans="1:5">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A66" s="3" t="s">
         <v>144</v>
       </c>
@@ -2439,7 +2445,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="67" spans="1:5">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A67" s="3" t="s">
         <v>144</v>
       </c>
@@ -2456,7 +2462,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="68" spans="1:5">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A68" s="3" t="s">
         <v>144</v>
       </c>
@@ -2473,7 +2479,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="69" spans="1:5">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A69" s="3" t="s">
         <v>144</v>
       </c>
@@ -2490,7 +2496,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="70" spans="1:5">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A70" s="3" t="s">
         <v>144</v>
       </c>
@@ -2507,7 +2513,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="71" spans="1:5">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A71" s="3" t="s">
         <v>144</v>
       </c>
@@ -2524,7 +2530,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="72" spans="1:5">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>168</v>
       </c>
@@ -2541,7 +2547,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="73" spans="1:5">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>168</v>
       </c>
@@ -2558,7 +2564,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="74" spans="1:5">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>168</v>
       </c>
@@ -2575,7 +2581,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="75" spans="1:5">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>168</v>
       </c>
@@ -2592,7 +2598,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="76" spans="1:5">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>168</v>
       </c>
@@ -2609,7 +2615,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="77" spans="1:5">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>168</v>
       </c>
@@ -2626,7 +2632,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="78" spans="1:5">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A78" s="2" t="s">
         <v>182</v>
       </c>
@@ -2643,7 +2649,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="79" spans="1:5">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A79" s="2" t="s">
         <v>182</v>
       </c>
@@ -2660,7 +2666,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="80" spans="1:5">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A80" s="2" t="s">
         <v>182</v>
       </c>
@@ -2677,7 +2683,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="81" spans="1:5">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A81" s="2" t="s">
         <v>182</v>
       </c>
@@ -2694,7 +2700,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="82" spans="1:5">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A82" s="2" t="s">
         <v>182</v>
       </c>
@@ -2711,7 +2717,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="83" spans="1:5">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A83" s="2" t="s">
         <v>182</v>
       </c>
@@ -2728,7 +2734,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="84" spans="1:5">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A84" s="2" t="s">
         <v>182</v>
       </c>
@@ -2745,7 +2751,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="85" spans="1:5">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A85" s="2" t="s">
         <v>182</v>
       </c>
@@ -2762,7 +2768,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="86" spans="1:5">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A86" s="2" t="s">
         <v>182</v>
       </c>
@@ -2779,7 +2785,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="87" spans="1:5">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A87" s="2" t="s">
         <v>182</v>
       </c>
@@ -2796,7 +2802,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="88" spans="1:5">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A88" s="2" t="s">
         <v>182</v>
       </c>
@@ -2813,7 +2819,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="89" spans="1:5">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A89" s="2" t="s">
         <v>182</v>
       </c>
@@ -2830,7 +2836,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="90" spans="1:5">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A90" s="2" t="s">
         <v>182</v>
       </c>
@@ -2847,7 +2853,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="91" spans="1:5">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A91" s="2" t="s">
         <v>182</v>
       </c>
@@ -2864,7 +2870,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="92" spans="1:5">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>217</v>
       </c>
@@ -2881,7 +2887,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="93" spans="1:5">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>217</v>
       </c>
@@ -2898,7 +2904,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="94" spans="1:5">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>217</v>
       </c>
@@ -2915,7 +2921,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="95" spans="1:5">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>217</v>
       </c>
@@ -2932,7 +2938,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="96" spans="1:5">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>217</v>
       </c>
@@ -2949,7 +2955,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="97" spans="1:5">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>217</v>
       </c>
@@ -2966,7 +2972,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="98" spans="1:5">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>217</v>
       </c>
@@ -2983,7 +2989,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="99" spans="1:5">
+    <row r="99" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>217</v>
       </c>
@@ -3000,7 +3006,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="100" spans="1:5">
+    <row r="100" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>217</v>
       </c>
@@ -3017,7 +3023,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="101" spans="1:5">
+    <row r="101" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>217</v>
       </c>
@@ -3034,7 +3040,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="102" spans="1:5">
+    <row r="102" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
         <v>217</v>
       </c>
@@ -3051,7 +3057,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="103" spans="1:5">
+    <row r="103" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
         <v>217</v>
       </c>
@@ -3068,7 +3074,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="104" spans="1:5">
+    <row r="104" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
         <v>217</v>
       </c>
@@ -3085,7 +3091,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="105" spans="1:5">
+    <row r="105" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
         <v>217</v>
       </c>
@@ -3102,7 +3108,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="106" spans="1:5">
+    <row r="106" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
         <v>217</v>
       </c>
@@ -3119,7 +3125,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="107" spans="1:5">
+    <row r="107" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
         <v>217</v>
       </c>
@@ -3136,7 +3142,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="108" spans="1:5">
+    <row r="108" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
         <v>217</v>
       </c>
@@ -3153,7 +3159,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="109" spans="1:5">
+    <row r="109" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
         <v>217</v>
       </c>
@@ -3161,16 +3167,16 @@
         <v>254</v>
       </c>
       <c r="C109" t="s">
-        <v>255</v>
+        <v>275</v>
       </c>
       <c r="D109" t="s">
         <v>11</v>
       </c>
       <c r="E109" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="110" spans="1:5">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
         <v>217</v>
       </c>
@@ -3178,16 +3184,16 @@
         <v>254</v>
       </c>
       <c r="C110" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="D110" t="s">
         <v>11</v>
       </c>
       <c r="E110" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="111" spans="1:5">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
         <v>217</v>
       </c>
@@ -3195,16 +3201,16 @@
         <v>254</v>
       </c>
       <c r="C111" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="D111" t="s">
         <v>11</v>
       </c>
       <c r="E111" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="112" spans="1:5">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
         <v>217</v>
       </c>
@@ -3212,16 +3218,16 @@
         <v>254</v>
       </c>
       <c r="C112" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="D112" t="s">
         <v>11</v>
       </c>
       <c r="E112" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="113" spans="1:5">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
         <v>217</v>
       </c>
@@ -3229,143 +3235,140 @@
         <v>254</v>
       </c>
       <c r="C113" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="D113" t="s">
         <v>11</v>
       </c>
       <c r="E113" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="114" spans="1:5">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
         <v>217</v>
       </c>
       <c r="B114" t="s">
-        <v>254</v>
+        <v>263</v>
       </c>
       <c r="C114" t="s">
+        <v>264</v>
+      </c>
+      <c r="D114" t="s">
+        <v>11</v>
+      </c>
+      <c r="E114" s="4" t="s">
         <v>265</v>
       </c>
-      <c r="D114" t="s">
-        <v>11</v>
-      </c>
-      <c r="E114" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="115" spans="1:5">
+    </row>
+    <row r="115" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
         <v>217</v>
       </c>
       <c r="B115" t="s">
-        <v>254</v>
+        <v>263</v>
       </c>
       <c r="C115" t="s">
+        <v>266</v>
+      </c>
+      <c r="D115" t="s">
+        <v>11</v>
+      </c>
+      <c r="E115" s="4" t="s">
         <v>267</v>
       </c>
-      <c r="D115" t="s">
-        <v>11</v>
-      </c>
-      <c r="E115" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="116" spans="1:5">
+    </row>
+    <row r="116" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
         <v>217</v>
       </c>
       <c r="B116" t="s">
-        <v>254</v>
+        <v>263</v>
       </c>
       <c r="C116" t="s">
+        <v>268</v>
+      </c>
+      <c r="E116" s="4" t="s">
         <v>269</v>
       </c>
-      <c r="D116" t="s">
-        <v>11</v>
-      </c>
-      <c r="E116" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="117" spans="1:5">
+    </row>
+    <row r="117" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
         <v>217</v>
       </c>
       <c r="B117" t="s">
+        <v>263</v>
+      </c>
+      <c r="C117" t="s">
+        <v>270</v>
+      </c>
+      <c r="D117" t="s">
+        <v>11</v>
+      </c>
+      <c r="E117" s="4" t="s">
         <v>271</v>
       </c>
-      <c r="C117" t="s">
-        <v>272</v>
-      </c>
-      <c r="D117" t="s">
-        <v>11</v>
-      </c>
-      <c r="E117" s="4" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="118" spans="1:5">
+    </row>
+    <row r="118" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
         <v>217</v>
       </c>
       <c r="B118" t="s">
-        <v>271</v>
+        <v>277</v>
       </c>
       <c r="C118" t="s">
-        <v>274</v>
+        <v>280</v>
       </c>
       <c r="D118" t="s">
         <v>11</v>
       </c>
-      <c r="E118" s="4" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="119" spans="1:5">
+      <c r="E118" s="9" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="119" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
         <v>217</v>
       </c>
       <c r="B119" t="s">
-        <v>271</v>
+        <v>277</v>
       </c>
       <c r="C119" t="s">
-        <v>276</v>
+        <v>278</v>
       </c>
       <c r="D119" t="s">
         <v>11</v>
       </c>
-      <c r="E119" s="4" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="120" spans="1:5">
+      <c r="E119" s="9" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="120" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
         <v>217</v>
       </c>
       <c r="B120" t="s">
-        <v>271</v>
+        <v>277</v>
       </c>
       <c r="C120" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="D120" t="s">
         <v>11</v>
       </c>
-      <c r="E120" s="4" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="121" spans="1:5">
+      <c r="E120" s="9" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="121" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
-        <v>280</v>
+        <v>272</v>
       </c>
       <c r="C121" t="s">
-        <v>281</v>
+        <v>273</v>
       </c>
       <c r="D121" t="s">
-        <v>282</v>
+        <v>274</v>
       </c>
     </row>
   </sheetData>
@@ -3377,10 +3380,10 @@
   <hyperlinks>
     <hyperlink ref="E70" r:id="rId1" xr:uid="{EDABF343-D836-4711-A5DA-9962405EC1E7}"/>
     <hyperlink ref="E71" r:id="rId2" xr:uid="{8B725C0B-7E29-4A3F-899E-1EBE8A4D48FD}"/>
-    <hyperlink ref="E117" r:id="rId3" xr:uid="{083D8C29-2A7B-4E6D-B7AA-832F01A1669A}"/>
-    <hyperlink ref="E118" r:id="rId4" xr:uid="{177A0ED9-418A-458A-9CBB-A67744F1E99C}"/>
-    <hyperlink ref="E119" r:id="rId5" xr:uid="{EA2E8905-2966-4DB7-B61E-A39963CBC5F5}"/>
-    <hyperlink ref="E120" r:id="rId6" xr:uid="{FA6F529C-8BD7-4BDB-BEB4-016C3217CD81}"/>
+    <hyperlink ref="E114" r:id="rId3" xr:uid="{083D8C29-2A7B-4E6D-B7AA-832F01A1669A}"/>
+    <hyperlink ref="E115" r:id="rId4" xr:uid="{177A0ED9-418A-458A-9CBB-A67744F1E99C}"/>
+    <hyperlink ref="E116" r:id="rId5" xr:uid="{EA2E8905-2966-4DB7-B61E-A39963CBC5F5}"/>
+    <hyperlink ref="E117" r:id="rId6" xr:uid="{FA6F529C-8BD7-4BDB-BEB4-016C3217CD81}"/>
     <hyperlink ref="E78" r:id="rId7" xr:uid="{7AEB891E-B58E-44AF-8449-C0CE194ECE01}"/>
     <hyperlink ref="E82" r:id="rId8" xr:uid="{61658A60-B0B7-4BC6-B3DE-6D6DE86D3AAC}"/>
     <hyperlink ref="E83" r:id="rId9" xr:uid="{45B57624-339E-4B54-B328-743548B93950}"/>
@@ -3429,6 +3432,9 @@
     <hyperlink ref="E48" r:id="rId52" xr:uid="{6EB98AB0-4BDC-4A0A-B3B8-E8BB5DE04C24}"/>
     <hyperlink ref="E50" r:id="rId53" xr:uid="{D33CC655-09F2-4FDD-9489-02AC65B8E7D9}"/>
     <hyperlink ref="E49" r:id="rId54" xr:uid="{E8B78230-361A-413D-A920-F3B7FE1EE9DE}"/>
+    <hyperlink ref="E118" r:id="rId55" xr:uid="{E225BDA3-ABC6-954E-B270-9011E638606B}"/>
+    <hyperlink ref="E119" r:id="rId56" xr:uid="{F22C5809-B387-EC4F-85DC-26991D4D3F1B}"/>
+    <hyperlink ref="E120" r:id="rId57" xr:uid="{7C4D9899-D652-4A42-B2A6-29A203F7CA6B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>